<commit_message>
Can grab screenshots now
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,22 +424,432 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Producer</t>
+          <t>00:00:00.04</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Operator</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>job</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>notes</t>
+          <t>screenshot_00_00_00.04.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>00:00:02.07</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_02.07.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>00:00:05.06</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_05.06.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>00:00:10.23</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_10.23.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>00:00:15.08</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_15.08.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>00:00:18.20</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_18.20.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>00:00:24.02</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_24.02.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>00:00:28.06</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_28.06.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>00:00:30.18</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_30.18.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>00:00:34.20</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_34.20.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>00:00:42.03</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_42.03.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>00:00:48.04</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_48.04.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>00:00:56.01</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_56.01.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>00:01:13.15</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>screenshot_00_01_13.15.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>00:00:00.04</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_00.04.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>00:00:02.07</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_02.07.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>00:00:05.06</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_05.06.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>00:00:10.23</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_10.23.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>00:00:15.08</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_15.08.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>00:00:18.20</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_18.20.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>00:00:24.02</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_24.02.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>00:00:28.06</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_28.06.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>00:00:30.18</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_30.18.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>00:00:34.20</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_34.20.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>00:00:42.03</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_42.03.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>00:00:48.04</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_48.04.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>00:00:56.01</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_56.01.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>00:01:13.15</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>screenshot_00_01_13.15.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>00:00:06.11</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_06.11.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>00:00:42.15</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_42.15.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>00:00:48.08</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_48.08.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>00:00:52.12</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_52.12.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>00:00:54.14</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_54.14.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>00:01:02.12</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>screenshot_00_01_02.12.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>00:00:00.01</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_00.01.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>00:00:42.02</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>screenshot_00_00_42.02.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>